<commit_message>
expaded readme files, added image of thrust vane data, and updated thrust vane spreadsheet to make everything easier to read
</commit_message>
<xml_diff>
--- a/thrustVanaAnalisis/thrustVaneLift.xlsx
+++ b/thrustVanaAnalisis/thrustVaneLift.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hudso\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hudso\Documents\UAV_REPO\thrustVanaAnalisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{827BEBB2-CF33-4A9C-9526-1629A755A2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA236160-90CF-403E-8BB0-D1A583AF86BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B32AE1CA-4528-4135-8D07-0FB96BD435F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>lift</t>
   </si>
@@ -71,39 +71,12 @@
   <si>
     <t>0m/s</t>
   </si>
-  <si>
-    <t>Y lift</t>
-  </si>
-  <si>
-    <t>X AoA</t>
-  </si>
-  <si>
-    <t>Z air speed</t>
-  </si>
-  <si>
-    <t>2deg</t>
-  </si>
-  <si>
-    <t>0deg</t>
-  </si>
-  <si>
-    <t>4deg</t>
-  </si>
-  <si>
-    <t>6deg</t>
-  </si>
-  <si>
-    <t>8deg</t>
-  </si>
-  <si>
-    <t>10deg</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +84,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +135,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -168,14 +154,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,8 +231,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.40671522309711289"/>
-          <c:y val="3.2407407407407406E-2"/>
+          <c:x val="0.11910919540229888"/>
+          <c:y val="2.4762214356232992E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1359,8 +1348,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.9130311413775983E-4"/>
-                  <c:y val="-0.13055995285184657"/>
+                  <c:x val="-2.7818330141164787E-2"/>
+                  <c:y val="-0.13838581597362132"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -6477,16 +6466,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6513,16 +6502,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6549,16 +6538,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>77289</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>124097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>458289</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>120287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6585,16 +6574,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>255814</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>174715</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6621,16 +6610,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>366849</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>23949</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>135527</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6657,16 +6646,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>375557</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>173628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>2177</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>116477</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6991,18 +6980,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB452CC-A1F0-41E3-94E5-F3B0DE5C5333}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:AH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="20" max="20" width="9" customWidth="1"/>
+    <col min="1" max="6" width="8.88671875" style="2"/>
+    <col min="7" max="34" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7019,17 +7009,8 @@
       <c r="F1" s="1">
         <v>0</v>
       </c>
-      <c r="T1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7046,17 +7027,8 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="T2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -7073,209 +7045,248 @@
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T3" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="9"/>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T4" t="s">
-        <v>17</v>
-      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T5" t="s">
-        <v>18</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T6" t="s">
-        <v>19</v>
-      </c>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>-6.3868999999999995E-2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>-3.15E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="T7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>-5.6147000000000002E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-3.2300000000000002E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="9"/>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
+        <v>-0.13705000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>-6.6799999999999998E-2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>-6.3399999999999998E-2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>-3.4500000000000003E-2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4">
         <v>20</v>
       </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="9"/>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-0.22567999999999999</v>
+      </c>
+      <c r="C18" s="5">
+        <v>-0.1085</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2">
-        <v>-5.6147000000000002E-2</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-3.2300000000000002E-2</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="B19" s="5">
+        <v>-7.3894000000000001E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-3.9300000000000002E-2</v>
+      </c>
+      <c r="D19" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="B20" s="5">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5">
+        <v>20</v>
+      </c>
+      <c r="D20" s="5">
         <v>0</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="9"/>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="5">
-        <v>-0.13705000000000001</v>
-      </c>
-      <c r="C12" s="5">
-        <v>-6.6799999999999998E-2</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5">
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5">
-        <v>-6.3399999999999998E-2</v>
-      </c>
-      <c r="C13" s="5">
-        <v>-3.4500000000000003E-2</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="5">
-        <v>29</v>
-      </c>
-      <c r="C14" s="5">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="4">
-        <v>-0.22567999999999999</v>
-      </c>
-      <c r="C18" s="4">
-        <v>-0.1085</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4">
-        <v>-7.3894000000000001E-2</v>
-      </c>
-      <c r="C19" s="4">
-        <v>-3.9300000000000002E-2</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="4">
-        <v>29</v>
-      </c>
-      <c r="C20" s="4">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>0</v>
       </c>
@@ -7293,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
@@ -7311,7 +7322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
@@ -7329,69 +7340,133 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="9"/>
+      <c r="C26" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="7">
         <v>-0.480985</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="7">
         <v>-0.2331</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="7">
         <v>0</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3">
+      <c r="E29" s="7"/>
+      <c r="F29" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="7">
         <v>-0.21228</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="7">
         <v>-7.22E-2</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="7">
         <v>0</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3">
+      <c r="E30" s="7"/>
+      <c r="F30" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="7">
         <v>20</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="7">
         <v>0</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3">
+      <c r="E31" s="7"/>
+      <c r="F31" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="9"/>
+      <c r="C32" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>